<commit_message>
[#9ct19v] - Added new sources and fixed upload of indicators
</commit_message>
<xml_diff>
--- a/src/test/resources/Indicators.xlsx
+++ b/src/test/resources/Indicators.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t xml:space="preserve">Level</t>
   </si>
@@ -77,9 +77,6 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Project's M&amp;E System</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
     <t xml:space="preserve">Number and percentage of displacement sites in urban areas receiving urban site management services.</t>
   </si>
   <si>
+    <t xml:space="preserve">OCHA Indicator Registry, FAO</t>
+  </si>
+  <si>
     <t xml:space="preserve">changed</t>
   </si>
   <si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t xml:space="preserve">Estimated number and percentage of displaced persons in displacement sites without documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCHA Indicator Registry, Capacity4Dev</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L6:L8"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,14 +447,14 @@
       <c r="H2" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,10 +465,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
@@ -476,14 +479,14 @@
       <c r="H3" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,185 +497,185 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>720</v>
-      </c>
-      <c r="I9" s="1" t="s">
+        <v>720.998</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>39</v>
@@ -680,10 +683,10 @@
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>40</v>
@@ -692,19 +695,19 @@
         <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>720</v>
-      </c>
-      <c r="I10" s="1" t="s">
+        <v>720.112</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>39</v>
@@ -1154,7 +1157,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L6:L8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>